<commit_message>
Fixed model's faces. Start working on texture 2D
</commit_message>
<xml_diff>
--- a/Docs/Model.xlsx
+++ b/Docs/Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Рабочий стол\CG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431F116-004E-4135-BFD6-A4AA6561C53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562DD30D-928D-4139-AA50-911E589A828E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
   <si>
     <t>Vertex List</t>
   </si>
@@ -71,15 +71,34 @@
   <si>
     <t>GT</t>
   </si>
+  <si>
+    <t>cw</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>acw</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -231,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -248,11 +267,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -908,24 +948,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B39653B9-F65D-4510-A104-AB7A2E9C98B6}" name="Table6" displayName="Table6" ref="U5:X18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B39653B9-F65D-4510-A104-AB7A2E9C98B6}" name="Table6" displayName="Table6" ref="U5:X18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{80725753-44E0-4CC8-B5AD-90D7C78005FF}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{6656755C-FCB1-41A0-81C2-2CF4AF04CAC3}" name="Column2" headerRowDxfId="4" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{8D5A3070-F670-4079-A227-74F5FE046430}" name="Column3" headerRowDxfId="5" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{516D5E11-5895-4856-85B2-F36CF577AF40}" name="Column4" headerRowDxfId="6" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6656755C-FCB1-41A0-81C2-2CF4AF04CAC3}" name="Column2" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{8D5A3070-F670-4079-A227-74F5FE046430}" name="Column3" headerRowDxfId="12" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{516D5E11-5895-4856-85B2-F36CF577AF40}" name="Column4" headerRowDxfId="10" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9ED4482C-2132-4C5A-95A5-18B500C39B43}" name="Table7910" displayName="Table7910" ref="U21:X42" headerRowCount="0" totalsRowShown="0" dataDxfId="3">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9ED4482C-2132-4C5A-95A5-18B500C39B43}" name="Table7910" displayName="Table7910" ref="U21:AC42" headerRowCount="0" totalsRowShown="0" dataDxfId="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E2B410FE-E65E-42B2-919C-47D779EFE0BB}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{39E2A25B-D1B8-46F6-A445-02D2B4DDB7A4}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{6C72FAEB-5386-4857-9F53-ECDA861E2D3A}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D534591A-44DF-41B9-BD65-F1105A70947A}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{39E2A25B-D1B8-46F6-A445-02D2B4DDB7A4}" name="Column2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6C72FAEB-5386-4857-9F53-ECDA861E2D3A}" name="Column3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D534591A-44DF-41B9-BD65-F1105A70947A}" name="Column4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{47021E41-967E-4103-8A36-66D889FF05D1}" name="Column5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{23D49E50-6BA3-4052-8D96-BE72B805F0EA}" name="Column6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{874DD091-B08D-471E-9E76-8AD6F7F64B93}" name="Column7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{C0C3A9E0-832F-41FA-A085-C8AA364B0E14}" name="Column8" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{A6AB3976-83E8-45DE-A1D3-EEA79472E587}" name="Column9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1194,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:AC43"/>
+  <dimension ref="C4:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="114" workbookViewId="0">
+      <selection activeCell="AC42" sqref="Z21:AC42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.21875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1212,7 +1257,7 @@
     <col min="28" max="29" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J4">
         <v>5</v>
       </c>
@@ -1220,7 +1265,13 @@
       <c r="W4"/>
       <c r="X4"/>
     </row>
-    <row r="5" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="K5" s="2"/>
       <c r="M5">
         <v>4</v>
@@ -1229,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K6" s="1"/>
       <c r="V6" s="6" t="s">
         <v>1</v>
@@ -1244,7 +1295,10 @@
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="U7">
         <v>0</v>
@@ -1262,7 +1316,7 @@
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
     </row>
-    <row r="8" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K8" s="1"/>
       <c r="U8">
         <v>1</v>
@@ -1280,7 +1334,7 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="10:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K9" s="1"/>
       <c r="L9">
         <v>3</v>
@@ -1304,7 +1358,7 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
     </row>
-    <row r="10" spans="10:29" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:29" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1325,9 +1379,12 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="10:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J11">
         <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -1348,7 +1405,7 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
     </row>
-    <row r="12" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="U12">
         <v>5</v>
       </c>
@@ -1365,7 +1422,7 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J13">
         <v>11</v>
       </c>
@@ -1385,7 +1442,13 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
     </row>
-    <row r="14" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="K14" s="2"/>
       <c r="M14">
         <v>10</v>
@@ -1406,7 +1469,7 @@
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K15" s="1"/>
       <c r="U15">
         <v>8</v>
@@ -1424,7 +1487,10 @@
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
     </row>
-    <row r="16" spans="10:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="U16">
         <v>9</v>
@@ -1442,7 +1508,7 @@
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K17" s="1"/>
       <c r="U17">
         <v>10</v>
@@ -1460,7 +1526,7 @@
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
     </row>
-    <row r="18" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K18" s="1"/>
       <c r="L18">
         <v>9</v>
@@ -1484,7 +1550,7 @@
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="4:29" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:29" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -1495,9 +1561,12 @@
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
     </row>
-    <row r="20" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J20">
         <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>8</v>
       </c>
       <c r="O20">
         <v>7</v>
@@ -1508,17 +1577,19 @@
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="V21" t="s">
         <v>4</v>
       </c>
       <c r="W21"/>
       <c r="X21"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
     </row>
-    <row r="22" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D22">
         <v>2</v>
       </c>
@@ -1540,11 +1611,16 @@
       <c r="X22" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
       <c r="K23" s="7"/>
@@ -1561,15 +1637,22 @@
       <c r="X23" s="6">
         <v>4</v>
       </c>
+      <c r="Y23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
     </row>
-    <row r="24" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="3"/>
       <c r="F24" s="9"/>
       <c r="K24" s="3"/>
       <c r="L24" s="9"/>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
       <c r="U24" t="s">
         <v>5</v>
       </c>
@@ -1582,11 +1665,15 @@
       <c r="X24" s="6">
         <v>3</v>
       </c>
+      <c r="Y24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>1</v>
       </c>
@@ -1611,11 +1698,15 @@
       <c r="X25" s="6">
         <v>2</v>
       </c>
+      <c r="Y25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
     </row>
-    <row r="26" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U26" t="s">
         <v>6</v>
       </c>
@@ -1628,11 +1719,15 @@
       <c r="X26" s="6">
         <v>1</v>
       </c>
+      <c r="Y26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z26" s="6"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
     </row>
-    <row r="27" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>5</v>
       </c>
@@ -1661,8 +1756,15 @@
       <c r="X27" s="6">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+    </row>
+    <row r="28" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
       <c r="K28" s="10"/>
@@ -1679,8 +1781,18 @@
       <c r="X28" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+    </row>
+    <row r="29" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="K29" s="10"/>
@@ -1697,12 +1809,22 @@
       <c r="X29" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+    </row>
+    <row r="30" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="K30" s="10"/>
       <c r="L30" s="11"/>
+      <c r="M30" t="s">
+        <v>10</v>
+      </c>
       <c r="U30" t="s">
         <v>8</v>
       </c>
@@ -1715,8 +1837,15 @@
       <c r="X30" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+    </row>
+    <row r="31" spans="3:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="K31" s="10"/>
@@ -1733,8 +1862,23 @@
       <c r="X31" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z31" s="6">
+        <v>4</v>
+      </c>
+      <c r="AA31" s="6">
+        <v>10</v>
+      </c>
+      <c r="AB31" s="6">
+        <v>11</v>
+      </c>
+      <c r="AC31" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="3:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E32" s="3"/>
       <c r="F32" s="9"/>
       <c r="K32" s="3"/>
@@ -1751,8 +1895,23 @@
       <c r="X32" s="6">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="4:24" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z32" s="6">
+        <v>4</v>
+      </c>
+      <c r="AA32" s="6">
+        <v>11</v>
+      </c>
+      <c r="AB32" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D33">
         <v>0</v>
       </c>
@@ -1777,8 +1936,23 @@
       <c r="X33" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="4:24" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z33" s="6">
+        <v>3</v>
+      </c>
+      <c r="AA33" s="6">
+        <v>10</v>
+      </c>
+      <c r="AB33" s="6">
+        <v>4</v>
+      </c>
+      <c r="AC33" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="U34" t="s">
         <v>10</v>
       </c>
@@ -1791,8 +1965,23 @@
       <c r="X34" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="4:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z34" s="6">
+        <v>3</v>
+      </c>
+      <c r="AA34" s="6">
+        <v>9</v>
+      </c>
+      <c r="AB34" s="6">
+        <v>10</v>
+      </c>
+      <c r="AC34" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H35">
         <v>9</v>
       </c>
@@ -1811,8 +2000,18 @@
       <c r="X35" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="4:24" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+    </row>
+    <row r="36" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>14</v>
+      </c>
       <c r="I36" s="7"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -1829,8 +2028,15 @@
       <c r="X36" s="6">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="4:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6"/>
+    </row>
+    <row r="37" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I37" s="3"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
@@ -1839,16 +2045,31 @@
         <v>14</v>
       </c>
       <c r="V37" s="6">
+        <v>2</v>
+      </c>
+      <c r="W37" s="6">
         <v>3</v>
       </c>
-      <c r="W37" s="6">
+      <c r="X37" s="6">
         <v>9</v>
       </c>
-      <c r="X37" s="6">
+      <c r="Y37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z37" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA37" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="4:24" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AB37" s="6">
+        <v>9</v>
+      </c>
+      <c r="AC37" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="H38">
         <v>3</v>
       </c>
@@ -1859,16 +2080,32 @@
         <v>14</v>
       </c>
       <c r="V38" s="6">
+        <v>2</v>
+      </c>
+      <c r="W38" s="6">
+        <v>9</v>
+      </c>
+      <c r="X38" s="6">
+        <v>8</v>
+      </c>
+      <c r="Y38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z38" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA38" s="6">
+        <v>9</v>
+      </c>
+      <c r="AB38" s="6">
         <v>3</v>
       </c>
-      <c r="W38" s="6">
-        <v>8</v>
-      </c>
-      <c r="X38" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="4:24" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC38" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="4:29" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T39" s="15"/>
       <c r="U39" t="s">
         <v>13</v>
       </c>
@@ -1881,8 +2118,15 @@
       <c r="X39" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="4:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6"/>
+      <c r="AC39" s="6"/>
+    </row>
+    <row r="40" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H40">
         <v>6</v>
       </c>
@@ -1901,8 +2145,18 @@
       <c r="X40" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="4:24" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y40" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
+      <c r="AB40" s="6"/>
+      <c r="AC40" s="6"/>
+    </row>
+    <row r="41" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
       <c r="I41" s="7"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -1919,8 +2173,23 @@
       <c r="X41" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="4:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z41" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="6">
+        <v>8</v>
+      </c>
+      <c r="AB41" s="6">
+        <v>2</v>
+      </c>
+      <c r="AC41" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="4:29" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I42" s="3"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -1937,8 +2206,23 @@
       <c r="X42" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="4:24" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z42" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="6">
+        <v>7</v>
+      </c>
+      <c r="AB42" s="6">
+        <v>8</v>
+      </c>
+      <c r="AC42" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="4:29" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="H43">
         <v>0</v>
       </c>
@@ -1947,6 +2231,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D14:G14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>